<commit_message>
fix csv and finish graben toy model
</commit_message>
<xml_diff>
--- a/data/graben_test_interfaces.xlsx
+++ b/data/graben_test_interfaces.xlsx
@@ -8,27 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nijan/Documents/git/PCT-modelling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0EC7A30-5E11-9047-9619-7AB8281EFBB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DAEB8C-0DF9-6F46-B905-3B2F76F5E2FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="6460" windowWidth="27240" windowHeight="16440" xr2:uid="{BBDAB484-6321-5F4D-B84E-6FA262CC49F4}"/>
+    <workbookView xWindow="7700" yWindow="2040" windowWidth="31440" windowHeight="20640" xr2:uid="{BBDAB484-6321-5F4D-B84E-6FA262CC49F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$2:$B$28</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$2:$C$28</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$2:$C$28</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$28</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$28</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$2:$B$28</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$2:$C$28</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$2:$B$28</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="10">
   <si>
     <t>X</t>
   </si>
@@ -56,29 +42,41 @@
     <t>Z</t>
   </si>
   <si>
+    <t>sandstone</t>
+  </si>
+  <si>
+    <t>fault1</t>
+  </si>
+  <si>
+    <t>fault2</t>
+  </si>
+  <si>
+    <t>shale</t>
+  </si>
+  <si>
+    <t>limestone</t>
+  </si>
+  <si>
     <t>formation</t>
   </si>
   <si>
-    <t>sandstone</t>
-  </si>
-  <si>
-    <t>fault1</t>
-  </si>
-  <si>
-    <t>fault2</t>
-  </si>
-  <si>
-    <t>shale</t>
+    <t>shale2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -420,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68F792E-47A1-434D-8C3A-5C3A647C893D}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -439,7 +437,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -453,7 +451,7 @@
         <v>850</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -461,13 +459,13 @@
         <v>200</v>
       </c>
       <c r="B3">
-        <v>570</v>
+        <v>500</v>
       </c>
       <c r="C3">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -475,13 +473,13 @@
         <v>200</v>
       </c>
       <c r="B4">
-        <v>850</v>
+        <v>570</v>
       </c>
       <c r="C4">
-        <v>450</v>
+        <v>180</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -489,13 +487,13 @@
         <v>200</v>
       </c>
       <c r="B5">
-        <v>980</v>
+        <v>910</v>
       </c>
       <c r="C5">
-        <v>950</v>
+        <v>500</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -503,13 +501,13 @@
         <v>200</v>
       </c>
       <c r="B6">
-        <v>600</v>
+        <v>980</v>
       </c>
       <c r="C6">
-        <v>700</v>
+        <v>950</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -517,13 +515,13 @@
         <v>200</v>
       </c>
       <c r="B7">
-        <v>820</v>
+        <v>850</v>
       </c>
       <c r="C7">
-        <v>750</v>
+        <v>180</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -531,10 +529,10 @@
         <v>200</v>
       </c>
       <c r="B8">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="C8">
-        <v>920</v>
+        <v>700</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -545,10 +543,10 @@
         <v>200</v>
       </c>
       <c r="B9">
-        <v>1200</v>
+        <v>820</v>
       </c>
       <c r="C9">
-        <v>850</v>
+        <v>750</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -559,10 +557,10 @@
         <v>200</v>
       </c>
       <c r="B10">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="C10">
-        <v>830</v>
+        <v>920</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -573,10 +571,10 @@
         <v>200</v>
       </c>
       <c r="B11">
-        <v>200</v>
+        <v>1200</v>
       </c>
       <c r="C11">
-        <v>770</v>
+        <v>850</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -587,13 +585,13 @@
         <v>200</v>
       </c>
       <c r="B12">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="C12">
-        <v>500</v>
+        <v>830</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -601,13 +599,13 @@
         <v>200</v>
       </c>
       <c r="B13">
-        <v>820</v>
+        <v>200</v>
       </c>
       <c r="C13">
-        <v>530</v>
+        <v>770</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -615,13 +613,13 @@
         <v>200</v>
       </c>
       <c r="B14">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="C14">
-        <v>680</v>
+        <v>500</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -629,13 +627,13 @@
         <v>200</v>
       </c>
       <c r="B15">
-        <v>1200</v>
+        <v>820</v>
       </c>
       <c r="C15">
-        <v>650</v>
+        <v>530</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -643,13 +641,13 @@
         <v>200</v>
       </c>
       <c r="B16">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="C16">
-        <v>650</v>
+        <v>680</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -657,19 +655,216 @@
         <v>200</v>
       </c>
       <c r="B17">
-        <v>200</v>
+        <v>1200</v>
       </c>
       <c r="C17">
+        <v>650</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>200</v>
+      </c>
+      <c r="B18">
+        <v>400</v>
+      </c>
+      <c r="C18">
+        <v>650</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>200</v>
+      </c>
+      <c r="B19">
+        <v>200</v>
+      </c>
+      <c r="C19">
         <v>600</v>
       </c>
-      <c r="D17" t="s">
-        <v>4</v>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>200</v>
+      </c>
+      <c r="B20">
+        <v>200</v>
+      </c>
+      <c r="C20">
+        <v>320</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>200</v>
+      </c>
+      <c r="B21">
+        <v>400</v>
+      </c>
+      <c r="C21">
+        <v>350</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>200</v>
+      </c>
+      <c r="B22">
+        <v>600</v>
+      </c>
+      <c r="C22">
+        <v>200</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>200</v>
+      </c>
+      <c r="B23">
+        <v>820</v>
+      </c>
+      <c r="C23">
+        <v>230</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>200</v>
+      </c>
+      <c r="B24">
+        <v>1000</v>
+      </c>
+      <c r="C24">
+        <v>370</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>200</v>
+      </c>
+      <c r="B25">
+        <v>1200</v>
+      </c>
+      <c r="C25">
+        <v>350</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>200</v>
+      </c>
+      <c r="B26">
+        <v>200</v>
+      </c>
+      <c r="C26">
+        <v>900</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>200</v>
+      </c>
+      <c r="B27">
+        <v>400</v>
+      </c>
+      <c r="C27">
+        <v>895</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>200</v>
+      </c>
+      <c r="B28">
+        <v>600</v>
+      </c>
+      <c r="C28">
+        <v>900</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>200</v>
+      </c>
+      <c r="B29">
+        <v>820</v>
+      </c>
+      <c r="C29">
+        <v>905</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>200</v>
+      </c>
+      <c r="B30">
+        <v>1000</v>
+      </c>
+      <c r="C30">
+        <v>910</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>200</v>
+      </c>
+      <c r="B31">
+        <v>1200</v>
+      </c>
+      <c r="C31">
+        <v>910</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:D17">
     <sortCondition ref="D2:D17"/>
   </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>